<commit_message>
Removed some bugs from the code
</commit_message>
<xml_diff>
--- a/2023-10-01Sales.xlsx
+++ b/2023-10-01Sales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>PC</t>
   </si>
@@ -37,7 +37,7 @@
     <t>121212</t>
   </si>
   <si>
-    <t>2023-10-29</t>
+    <t>2023-10-31</t>
   </si>
   <si>
     <t>Caro White Cream</t>
@@ -46,16 +46,10 @@
     <t>1800</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3600</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>9000</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5400</t>
   </si>
 </sst>
 </file>
@@ -387,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,26 +427,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>